<commit_message>
added satellite option as comment
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ev693020\Github\Disaster-Modeling-Resilience\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAA9804-CB3A-496D-9351-4CAF2FF33DCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C451E8C1-C032-42E4-A196-089E648101B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31695" yWindow="2130" windowWidth="19785" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5850" yWindow="900" windowWidth="19785" windowHeight="13440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population_Community" sheetId="1" r:id="rId1"/>
@@ -1530,7 +1530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1540,7 +1540,6 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1824,7 +1823,7 @@
   <dimension ref="A1:T117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,7 +2429,7 @@
       <c r="A17" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -2467,7 +2466,7 @@
       <c r="A18" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -2504,7 +2503,7 @@
       <c r="A19" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -2541,7 +2540,7 @@
       <c r="A20" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -2578,7 +2577,7 @@
       <c r="A21" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -2615,7 +2614,7 @@
       <c r="A22" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -2652,7 +2651,7 @@
       <c r="A23" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="5" t="s">
+      <c r="B23" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -2689,7 +2688,7 @@
       <c r="A24" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -2726,7 +2725,7 @@
       <c r="A25" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="B25" s="2" t="s">
         <v>72</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -2763,7 +2762,7 @@
       <c r="A26" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B26" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -2800,7 +2799,7 @@
       <c r="A27" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2837,7 +2836,7 @@
       <c r="A28" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2874,7 +2873,7 @@
       <c r="A29" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B29" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -2911,7 +2910,7 @@
       <c r="A30" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -2948,7 +2947,7 @@
       <c r="A31" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B31" s="5" t="s">
+      <c r="B31" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -2985,7 +2984,7 @@
       <c r="A32" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="B32" s="5" t="s">
+      <c r="B32" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -3022,7 +3021,7 @@
       <c r="A33" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="2" t="s">
         <v>108</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -3059,7 +3058,7 @@
       <c r="A34" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -3096,7 +3095,7 @@
       <c r="A35" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -3133,7 +3132,7 @@
       <c r="A36" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="B36" s="5" t="s">
+      <c r="B36" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -3170,7 +3169,7 @@
       <c r="A37" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B37" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -3207,7 +3206,7 @@
       <c r="A38" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B38" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -3244,7 +3243,7 @@
       <c r="A39" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="B39" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -3281,7 +3280,7 @@
       <c r="A40" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="B40" s="5" t="s">
+      <c r="B40" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -3318,7 +3317,7 @@
       <c r="A41" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B41" s="5" t="s">
+      <c r="B41" s="2" t="s">
         <v>170</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -3355,7 +3354,7 @@
       <c r="A42" s="3" t="s">
         <v>171</v>
       </c>
-      <c r="B42" s="5" t="s">
+      <c r="B42" s="2" t="s">
         <v>203</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -3392,7 +3391,7 @@
       <c r="A43" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B43" s="5" t="s">
+      <c r="B43" s="2" t="s">
         <v>203</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -3429,7 +3428,7 @@
       <c r="A44" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="B44" s="5" t="s">
+      <c r="B44" s="2" t="s">
         <v>203</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -3466,7 +3465,7 @@
       <c r="A45" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="B45" s="5" t="s">
+      <c r="B45" s="2" t="s">
         <v>203</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -3503,7 +3502,7 @@
       <c r="A46" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B46" s="5" t="s">
+      <c r="B46" s="2" t="s">
         <v>203</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -3540,7 +3539,7 @@
       <c r="A47" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="2" t="s">
         <v>203</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -3577,7 +3576,7 @@
       <c r="A48" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="B48" s="5" t="s">
+      <c r="B48" s="2" t="s">
         <v>203</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -3614,7 +3613,7 @@
       <c r="A49" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="2" t="s">
         <v>203</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -3651,7 +3650,7 @@
       <c r="A50" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -3688,7 +3687,7 @@
       <c r="A51" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="B51" s="5" t="s">
+      <c r="B51" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -3725,7 +3724,7 @@
       <c r="A52" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="B52" s="5" t="s">
+      <c r="B52" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -3762,7 +3761,7 @@
       <c r="A53" s="3" t="s">
         <v>210</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -3799,7 +3798,7 @@
       <c r="A54" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -3836,7 +3835,7 @@
       <c r="A55" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="B55" s="5" t="s">
+      <c r="B55" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -3873,7 +3872,7 @@
       <c r="A56" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="B56" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -3910,7 +3909,7 @@
       <c r="A57" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="B57" s="2" t="s">
         <v>220</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -3947,7 +3946,7 @@
       <c r="A58" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="2" t="s">
         <v>238</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -3984,7 +3983,7 @@
       <c r="A59" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="2" t="s">
         <v>238</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -4021,7 +4020,7 @@
       <c r="A60" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B60" s="2" t="s">
         <v>238</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -4058,7 +4057,7 @@
       <c r="A61" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="B61" s="5" t="s">
+      <c r="B61" s="2" t="s">
         <v>238</v>
       </c>
       <c r="C61" s="3" t="s">
@@ -4095,7 +4094,7 @@
       <c r="A62" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="B62" s="2" t="s">
         <v>238</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -4132,7 +4131,7 @@
       <c r="A63" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="2" t="s">
         <v>238</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -4169,7 +4168,7 @@
       <c r="A64" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="2" t="s">
         <v>238</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -4206,7 +4205,7 @@
       <c r="A65" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="2" t="s">
         <v>238</v>
       </c>
       <c r="C65" s="3" t="s">
@@ -4243,7 +4242,7 @@
       <c r="A66" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="B66" s="5" t="s">
+      <c r="B66" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -4280,7 +4279,7 @@
       <c r="A67" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B67" s="5" t="s">
+      <c r="B67" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -4317,7 +4316,7 @@
       <c r="A68" s="3" t="s">
         <v>273</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -4354,7 +4353,7 @@
       <c r="A69" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="B69" s="5" t="s">
+      <c r="B69" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -4391,7 +4390,7 @@
       <c r="A70" s="3" t="s">
         <v>277</v>
       </c>
-      <c r="B70" s="5" t="s">
+      <c r="B70" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -4428,7 +4427,7 @@
       <c r="A71" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="B71" s="5" t="s">
+      <c r="B71" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C71" s="3" t="s">
@@ -4465,7 +4464,7 @@
       <c r="A72" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="B72" s="5" t="s">
+      <c r="B72" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -4502,7 +4501,7 @@
       <c r="A73" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="B73" s="5" t="s">
+      <c r="B73" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -4539,7 +4538,7 @@
       <c r="A74" s="3" t="s">
         <v>285</v>
       </c>
-      <c r="B74" s="5" t="s">
+      <c r="B74" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -4576,7 +4575,7 @@
       <c r="A75" s="3" t="s">
         <v>287</v>
       </c>
-      <c r="B75" s="5" t="s">
+      <c r="B75" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -4613,7 +4612,7 @@
       <c r="A76" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B76" s="5" t="s">
+      <c r="B76" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C76" s="3" t="s">
@@ -4650,7 +4649,7 @@
       <c r="A77" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="B77" s="5" t="s">
+      <c r="B77" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C77" s="3" t="s">
@@ -4687,7 +4686,7 @@
       <c r="A78" s="3" t="s">
         <v>293</v>
       </c>
-      <c r="B78" s="5" t="s">
+      <c r="B78" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -4724,7 +4723,7 @@
       <c r="A79" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="B79" s="5" t="s">
+      <c r="B79" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C79" s="3" t="s">
@@ -4761,7 +4760,7 @@
       <c r="A80" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="B80" s="5" t="s">
+      <c r="B80" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C80" s="3" t="s">
@@ -4798,7 +4797,7 @@
       <c r="A81" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="B81" s="5" t="s">
+      <c r="B81" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C81" s="3" t="s">
@@ -4835,7 +4834,7 @@
       <c r="A82" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="B82" s="5" t="s">
+      <c r="B82" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -4872,7 +4871,7 @@
       <c r="A83" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="B83" s="5" t="s">
+      <c r="B83" s="2" t="s">
         <v>305</v>
       </c>
       <c r="C83" s="3" t="s">
@@ -4909,7 +4908,7 @@
       <c r="A84" s="3" t="s">
         <v>341</v>
       </c>
-      <c r="B84" s="5" t="s">
+      <c r="B84" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C84" s="3" t="s">
@@ -4946,7 +4945,7 @@
       <c r="A85" s="3" t="s">
         <v>343</v>
       </c>
-      <c r="B85" s="5" t="s">
+      <c r="B85" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C85" s="3" t="s">
@@ -4983,7 +4982,7 @@
       <c r="A86" s="3" t="s">
         <v>345</v>
       </c>
-      <c r="B86" s="5" t="s">
+      <c r="B86" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -5020,7 +5019,7 @@
       <c r="A87" s="3" t="s">
         <v>347</v>
       </c>
-      <c r="B87" s="5" t="s">
+      <c r="B87" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C87" s="3" t="s">
@@ -5057,7 +5056,7 @@
       <c r="A88" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B88" s="5" t="s">
+      <c r="B88" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C88" s="3" t="s">
@@ -5094,7 +5093,7 @@
       <c r="A89" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="B89" s="5" t="s">
+      <c r="B89" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C89" s="3" t="s">
@@ -5131,7 +5130,7 @@
       <c r="A90" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="B90" s="5" t="s">
+      <c r="B90" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C90" s="3" t="s">
@@ -5168,7 +5167,7 @@
       <c r="A91" s="3" t="s">
         <v>355</v>
       </c>
-      <c r="B91" s="5" t="s">
+      <c r="B91" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -5205,7 +5204,7 @@
       <c r="A92" s="3" t="s">
         <v>357</v>
       </c>
-      <c r="B92" s="5" t="s">
+      <c r="B92" s="2" t="s">
         <v>342</v>
       </c>
       <c r="C92" s="3" t="s">
@@ -5242,7 +5241,7 @@
       <c r="A93" s="3" t="s">
         <v>376</v>
       </c>
-      <c r="B93" s="5" t="s">
+      <c r="B93" s="2" t="s">
         <v>377</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -5279,7 +5278,7 @@
       <c r="A94" s="3" t="s">
         <v>378</v>
       </c>
-      <c r="B94" s="5" t="s">
+      <c r="B94" s="2" t="s">
         <v>377</v>
       </c>
       <c r="C94" s="3" t="s">
@@ -5316,7 +5315,7 @@
       <c r="A95" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="B95" s="5" t="s">
+      <c r="B95" s="2" t="s">
         <v>377</v>
       </c>
       <c r="C95" s="3" t="s">
@@ -5353,7 +5352,7 @@
       <c r="A96" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="B96" s="5" t="s">
+      <c r="B96" s="2" t="s">
         <v>377</v>
       </c>
       <c r="C96" s="3" t="s">
@@ -5390,7 +5389,7 @@
       <c r="A97" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="B97" s="5" t="s">
+      <c r="B97" s="2" t="s">
         <v>377</v>
       </c>
       <c r="C97" s="3" t="s">
@@ -5416,7 +5415,7 @@
       <c r="A98" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="B98" s="5" t="s">
+      <c r="B98" s="2" t="s">
         <v>377</v>
       </c>
       <c r="C98" s="3" t="s">
@@ -5442,7 +5441,7 @@
       <c r="A99" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="B99" s="5" t="s">
+      <c r="B99" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C99" s="3" t="s">
@@ -5468,7 +5467,7 @@
       <c r="A100" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="B100" s="5" t="s">
+      <c r="B100" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C100" s="3" t="s">
@@ -5494,7 +5493,7 @@
       <c r="A101" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="B101" s="5" t="s">
+      <c r="B101" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C101" s="3" t="s">
@@ -5520,7 +5519,7 @@
       <c r="A102" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="B102" s="5" t="s">
+      <c r="B102" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C102" s="3" t="s">
@@ -5546,7 +5545,7 @@
       <c r="A103" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="B103" s="5" t="s">
+      <c r="B103" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C103" s="3" t="s">
@@ -5572,7 +5571,7 @@
       <c r="A104" s="3" t="s">
         <v>410</v>
       </c>
-      <c r="B104" s="5" t="s">
+      <c r="B104" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C104" s="3" t="s">
@@ -5598,7 +5597,7 @@
       <c r="A105" s="3" t="s">
         <v>412</v>
       </c>
-      <c r="B105" s="5" t="s">
+      <c r="B105" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C105" s="3" t="s">
@@ -5624,7 +5623,7 @@
       <c r="A106" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="B106" s="5" t="s">
+      <c r="B106" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C106" s="3" t="s">
@@ -5650,7 +5649,7 @@
       <c r="A107" s="3" t="s">
         <v>416</v>
       </c>
-      <c r="B107" s="5" t="s">
+      <c r="B107" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C107" s="3" t="s">
@@ -5676,7 +5675,7 @@
       <c r="A108" s="3" t="s">
         <v>418</v>
       </c>
-      <c r="B108" s="5" t="s">
+      <c r="B108" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C108" s="3" t="s">
@@ -5702,7 +5701,7 @@
       <c r="A109" s="3" t="s">
         <v>420</v>
       </c>
-      <c r="B109" s="5" t="s">
+      <c r="B109" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C109" s="3" t="s">
@@ -5728,7 +5727,7 @@
       <c r="A110" s="3" t="s">
         <v>422</v>
       </c>
-      <c r="B110" s="5" t="s">
+      <c r="B110" s="2" t="s">
         <v>448</v>
       </c>
       <c r="C110" s="3" t="s">
@@ -5754,7 +5753,7 @@
       <c r="A111" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="B111" s="5" t="s">
+      <c r="B111" s="2" t="s">
         <v>450</v>
       </c>
       <c r="C111" s="3" t="s">
@@ -5780,7 +5779,7 @@
       <c r="A112" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="B112" s="5" t="s">
+      <c r="B112" s="2" t="s">
         <v>450</v>
       </c>
       <c r="C112" s="3" t="s">
@@ -5806,7 +5805,7 @@
       <c r="A113" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="B113" s="5" t="s">
+      <c r="B113" s="2" t="s">
         <v>450</v>
       </c>
       <c r="C113" s="3" t="s">
@@ -5832,7 +5831,7 @@
       <c r="A114" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="B114" s="5" t="s">
+      <c r="B114" s="2" t="s">
         <v>450</v>
       </c>
       <c r="C114" s="3" t="s">
@@ -5858,7 +5857,7 @@
       <c r="A115" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="B115" s="5" t="s">
+      <c r="B115" s="2" t="s">
         <v>450</v>
       </c>
       <c r="C115" s="3" t="s">
@@ -5884,7 +5883,7 @@
       <c r="A116" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="B116" s="5" t="s">
+      <c r="B116" s="2" t="s">
         <v>450</v>
       </c>
       <c r="C116" s="3" t="s">
@@ -5910,7 +5909,7 @@
       <c r="A117" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="B117" s="5" t="s">
+      <c r="B117" s="2" t="s">
         <v>450</v>
       </c>
       <c r="C117" s="3" t="s">

</xml_diff>

<commit_message>
Edited Xlsx & Added Harversine Function
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11027"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ev693020\Github\Disaster-Modeling-Resilience\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzovillafuerte/Documents/GitHub/Disaster-Modeling-Resilience/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69C0E892-7519-40C0-A6AF-DA7C3F66C527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64DDC983-934F-044D-9567-C252BB180600}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2490" yWindow="1035" windowWidth="19785" windowHeight="13440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2500" yWindow="1040" windowWidth="19780" windowHeight="13440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Population_Community" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="835" uniqueCount="528">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="527">
   <si>
     <t>location_id</t>
   </si>
@@ -1473,9 +1473,6 @@
     <t>13º19ʹ18"</t>
   </si>
   <si>
-    <t>Province</t>
-  </si>
-  <si>
     <t>Plaza Regocijo S/N</t>
   </si>
   <si>
@@ -1497,15 +1494,9 @@
     <t>latitude</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
     <t>13°31'00"S 71°58'48"W</t>
   </si>
   <si>
-    <t>Location</t>
-  </si>
-  <si>
     <t>13°35'04"S 72°03'31"W</t>
   </si>
   <si>
@@ -1561,9 +1552,6 @@
   </si>
   <si>
     <t>13°28'44"S 72°06'42"W</t>
-  </si>
-  <si>
-    <t>District</t>
   </si>
   <si>
     <t>13°27'19"S 72°15'19"W</t>
@@ -1626,6 +1614,15 @@
   </si>
   <si>
     <t>13°19'15"S 72°05'00"W</t>
+  </si>
+  <si>
+    <t>wh_id</t>
+  </si>
+  <si>
+    <t>address</t>
+  </si>
+  <si>
+    <t>location</t>
   </si>
 </sst>
 </file>
@@ -1635,7 +1632,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#\ ##0"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1668,14 +1665,9 @@
     </font>
     <font>
       <sz val="7"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
       <color indexed="8"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -1739,10 +1731,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2031,13 +2023,13 @@
       <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.140625" customWidth="1"/>
+    <col min="2" max="2" width="9.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2075,7 +2067,7 @@
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -2112,7 +2104,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>10</v>
       </c>
@@ -2149,7 +2141,7 @@
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
@@ -2186,7 +2178,7 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -2223,7 +2215,7 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>16</v>
       </c>
@@ -2260,7 +2252,7 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -2297,7 +2289,7 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -2334,7 +2326,7 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>22</v>
       </c>
@@ -2371,7 +2363,7 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>24</v>
       </c>
@@ -2408,7 +2400,7 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>26</v>
       </c>
@@ -2445,7 +2437,7 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -2482,7 +2474,7 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
@@ -2519,7 +2511,7 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>32</v>
       </c>
@@ -2556,7 +2548,7 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>34</v>
       </c>
@@ -2593,7 +2585,7 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>36</v>
       </c>
@@ -2630,7 +2622,7 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>71</v>
       </c>
@@ -2667,7 +2659,7 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>75</v>
       </c>
@@ -2704,7 +2696,7 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>79</v>
       </c>
@@ -2741,7 +2733,7 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>83</v>
       </c>
@@ -2778,7 +2770,7 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>87</v>
       </c>
@@ -2815,7 +2807,7 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>91</v>
       </c>
@@ -2852,7 +2844,7 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>95</v>
       </c>
@@ -2889,7 +2881,7 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>99</v>
       </c>
@@ -2926,7 +2918,7 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>103</v>
       </c>
@@ -2963,7 +2955,7 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>107</v>
       </c>
@@ -3000,7 +2992,7 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>109</v>
       </c>
@@ -3037,7 +3029,7 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>111</v>
       </c>
@@ -3074,7 +3066,7 @@
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>113</v>
       </c>
@@ -3111,7 +3103,7 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>115</v>
       </c>
@@ -3148,7 +3140,7 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>117</v>
       </c>
@@ -3185,7 +3177,7 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
         <v>119</v>
       </c>
@@ -3222,7 +3214,7 @@
       <c r="S32" s="1"/>
       <c r="T32" s="1"/>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
         <v>121</v>
       </c>
@@ -3259,7 +3251,7 @@
       <c r="S33" s="1"/>
       <c r="T33" s="1"/>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
         <v>138</v>
       </c>
@@ -3296,7 +3288,7 @@
       <c r="S34" s="1"/>
       <c r="T34" s="1"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
         <v>140</v>
       </c>
@@ -3333,7 +3325,7 @@
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>142</v>
       </c>
@@ -3370,7 +3362,7 @@
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
         <v>144</v>
       </c>
@@ -3407,7 +3399,7 @@
       <c r="S37" s="1"/>
       <c r="T37" s="1"/>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>146</v>
       </c>
@@ -3444,7 +3436,7 @@
       <c r="S38" s="1"/>
       <c r="T38" s="1"/>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
         <v>148</v>
       </c>
@@ -3481,7 +3473,7 @@
       <c r="S39" s="1"/>
       <c r="T39" s="1"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A40" s="3" t="s">
         <v>150</v>
       </c>
@@ -3518,7 +3510,7 @@
       <c r="S40" s="1"/>
       <c r="T40" s="1"/>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>152</v>
       </c>
@@ -3555,7 +3547,7 @@
       <c r="S41" s="1"/>
       <c r="T41" s="1"/>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>171</v>
       </c>
@@ -3592,7 +3584,7 @@
       <c r="S42" s="1"/>
       <c r="T42" s="1"/>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A43" s="3" t="s">
         <v>173</v>
       </c>
@@ -3629,7 +3621,7 @@
       <c r="S43" s="1"/>
       <c r="T43" s="1"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A44" s="3" t="s">
         <v>175</v>
       </c>
@@ -3666,7 +3658,7 @@
       <c r="S44" s="1"/>
       <c r="T44" s="1"/>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A45" s="3" t="s">
         <v>177</v>
       </c>
@@ -3703,7 +3695,7 @@
       <c r="S45" s="1"/>
       <c r="T45" s="1"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>179</v>
       </c>
@@ -3740,7 +3732,7 @@
       <c r="S46" s="1"/>
       <c r="T46" s="1"/>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>181</v>
       </c>
@@ -3777,7 +3769,7 @@
       <c r="S47" s="1"/>
       <c r="T47" s="1"/>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A48" s="3" t="s">
         <v>183</v>
       </c>
@@ -3814,7 +3806,7 @@
       <c r="S48" s="1"/>
       <c r="T48" s="1"/>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A49" s="3" t="s">
         <v>185</v>
       </c>
@@ -3851,7 +3843,7 @@
       <c r="S49" s="1"/>
       <c r="T49" s="1"/>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>204</v>
       </c>
@@ -3888,7 +3880,7 @@
       <c r="S50" s="1"/>
       <c r="T50" s="1"/>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A51" s="3" t="s">
         <v>206</v>
       </c>
@@ -3925,7 +3917,7 @@
       <c r="S51" s="1"/>
       <c r="T51" s="1"/>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A52" s="3" t="s">
         <v>208</v>
       </c>
@@ -3962,7 +3954,7 @@
       <c r="S52" s="1"/>
       <c r="T52" s="1"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A53" s="3" t="s">
         <v>210</v>
       </c>
@@ -3999,7 +3991,7 @@
       <c r="S53" s="1"/>
       <c r="T53" s="1"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>212</v>
       </c>
@@ -4036,7 +4028,7 @@
       <c r="S54" s="1"/>
       <c r="T54" s="1"/>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A55" s="3" t="s">
         <v>214</v>
       </c>
@@ -4073,7 +4065,7 @@
       <c r="S55" s="1"/>
       <c r="T55" s="1"/>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A56" s="3" t="s">
         <v>216</v>
       </c>
@@ -4110,7 +4102,7 @@
       <c r="S56" s="1"/>
       <c r="T56" s="1"/>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A57" s="3" t="s">
         <v>218</v>
       </c>
@@ -4147,7 +4139,7 @@
       <c r="S57" s="1"/>
       <c r="T57" s="1"/>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>237</v>
       </c>
@@ -4184,7 +4176,7 @@
       <c r="S58" s="1"/>
       <c r="T58" s="1"/>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A59" s="3" t="s">
         <v>239</v>
       </c>
@@ -4221,7 +4213,7 @@
       <c r="S59" s="1"/>
       <c r="T59" s="1"/>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>241</v>
       </c>
@@ -4258,7 +4250,7 @@
       <c r="S60" s="1"/>
       <c r="T60" s="1"/>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A61" s="3" t="s">
         <v>243</v>
       </c>
@@ -4295,7 +4287,7 @@
       <c r="S61" s="1"/>
       <c r="T61" s="1"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A62" s="3" t="s">
         <v>245</v>
       </c>
@@ -4332,7 +4324,7 @@
       <c r="S62" s="1"/>
       <c r="T62" s="1"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A63" s="3" t="s">
         <v>247</v>
       </c>
@@ -4369,7 +4361,7 @@
       <c r="S63" s="1"/>
       <c r="T63" s="1"/>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A64" s="3" t="s">
         <v>249</v>
       </c>
@@ -4406,7 +4398,7 @@
       <c r="S64" s="1"/>
       <c r="T64" s="1"/>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A65" s="3" t="s">
         <v>251</v>
       </c>
@@ -4443,7 +4435,7 @@
       <c r="S65" s="1"/>
       <c r="T65" s="1"/>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A66" s="3" t="s">
         <v>269</v>
       </c>
@@ -4480,7 +4472,7 @@
       <c r="S66" s="1"/>
       <c r="T66" s="1"/>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A67" s="3" t="s">
         <v>271</v>
       </c>
@@ -4517,7 +4509,7 @@
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A68" s="3" t="s">
         <v>273</v>
       </c>
@@ -4554,7 +4546,7 @@
       <c r="S68" s="1"/>
       <c r="T68" s="1"/>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>275</v>
       </c>
@@ -4591,7 +4583,7 @@
       <c r="S69" s="1"/>
       <c r="T69" s="1"/>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A70" s="3" t="s">
         <v>277</v>
       </c>
@@ -4628,7 +4620,7 @@
       <c r="S70" s="1"/>
       <c r="T70" s="1"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A71" s="3" t="s">
         <v>279</v>
       </c>
@@ -4665,7 +4657,7 @@
       <c r="S71" s="1"/>
       <c r="T71" s="1"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A72" s="3" t="s">
         <v>281</v>
       </c>
@@ -4702,7 +4694,7 @@
       <c r="S72" s="1"/>
       <c r="T72" s="1"/>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A73" s="3" t="s">
         <v>283</v>
       </c>
@@ -4739,7 +4731,7 @@
       <c r="S73" s="1"/>
       <c r="T73" s="1"/>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
         <v>285</v>
       </c>
@@ -4776,7 +4768,7 @@
       <c r="S74" s="1"/>
       <c r="T74" s="1"/>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A75" s="3" t="s">
         <v>287</v>
       </c>
@@ -4813,7 +4805,7 @@
       <c r="S75" s="1"/>
       <c r="T75" s="1"/>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A76" s="3" t="s">
         <v>289</v>
       </c>
@@ -4850,7 +4842,7 @@
       <c r="S76" s="1"/>
       <c r="T76" s="1"/>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A77" s="3" t="s">
         <v>291</v>
       </c>
@@ -4887,7 +4879,7 @@
       <c r="S77" s="1"/>
       <c r="T77" s="1"/>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A78" s="3" t="s">
         <v>293</v>
       </c>
@@ -4924,7 +4916,7 @@
       <c r="S78" s="1"/>
       <c r="T78" s="1"/>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A79" s="3" t="s">
         <v>295</v>
       </c>
@@ -4961,7 +4953,7 @@
       <c r="S79" s="1"/>
       <c r="T79" s="1"/>
     </row>
-    <row r="80" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>297</v>
       </c>
@@ -4998,7 +4990,7 @@
       <c r="S80" s="1"/>
       <c r="T80" s="1"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A81" s="3" t="s">
         <v>299</v>
       </c>
@@ -5035,7 +5027,7 @@
       <c r="S81" s="1"/>
       <c r="T81" s="1"/>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>301</v>
       </c>
@@ -5072,7 +5064,7 @@
       <c r="S82" s="1"/>
       <c r="T82" s="1"/>
     </row>
-    <row r="83" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20" ht="22" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>303</v>
       </c>
@@ -5109,7 +5101,7 @@
       <c r="S83" s="1"/>
       <c r="T83" s="1"/>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A84" s="3" t="s">
         <v>341</v>
       </c>
@@ -5146,7 +5138,7 @@
       <c r="S84" s="1"/>
       <c r="T84" s="1"/>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A85" s="3" t="s">
         <v>343</v>
       </c>
@@ -5183,7 +5175,7 @@
       <c r="S85" s="1"/>
       <c r="T85" s="1"/>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>345</v>
       </c>
@@ -5220,7 +5212,7 @@
       <c r="S86" s="1"/>
       <c r="T86" s="1"/>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A87" s="3" t="s">
         <v>347</v>
       </c>
@@ -5257,7 +5249,7 @@
       <c r="S87" s="1"/>
       <c r="T87" s="1"/>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A88" s="3" t="s">
         <v>349</v>
       </c>
@@ -5294,7 +5286,7 @@
       <c r="S88" s="1"/>
       <c r="T88" s="1"/>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A89" s="3" t="s">
         <v>351</v>
       </c>
@@ -5331,7 +5323,7 @@
       <c r="S89" s="1"/>
       <c r="T89" s="1"/>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>353</v>
       </c>
@@ -5368,7 +5360,7 @@
       <c r="S90" s="1"/>
       <c r="T90" s="1"/>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>355</v>
       </c>
@@ -5405,7 +5397,7 @@
       <c r="S91" s="1"/>
       <c r="T91" s="1"/>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A92" s="3" t="s">
         <v>357</v>
       </c>
@@ -5442,7 +5434,7 @@
       <c r="S92" s="1"/>
       <c r="T92" s="1"/>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A93" s="3" t="s">
         <v>376</v>
       </c>
@@ -5479,7 +5471,7 @@
       <c r="S93" s="1"/>
       <c r="T93" s="1"/>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A94" s="3" t="s">
         <v>378</v>
       </c>
@@ -5516,7 +5508,7 @@
       <c r="S94" s="1"/>
       <c r="T94" s="1"/>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A95" s="3" t="s">
         <v>380</v>
       </c>
@@ -5553,7 +5545,7 @@
       <c r="S95" s="1"/>
       <c r="T95" s="1"/>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A96" s="3" t="s">
         <v>382</v>
       </c>
@@ -5590,7 +5582,7 @@
       <c r="S96" s="1"/>
       <c r="T96" s="1"/>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" s="3" t="s">
         <v>384</v>
       </c>
@@ -5616,7 +5608,7 @@
         <v>8001</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" s="3" t="s">
         <v>386</v>
       </c>
@@ -5642,7 +5634,7 @@
         <v>4924</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" s="3" t="s">
         <v>400</v>
       </c>
@@ -5668,7 +5660,7 @@
         <v>12538</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" s="3" t="s">
         <v>402</v>
       </c>
@@ -5694,7 +5686,7 @@
         <v>7382</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" s="3" t="s">
         <v>404</v>
       </c>
@@ -5720,7 +5712,7 @@
         <v>2692</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>406</v>
       </c>
@@ -5746,7 +5738,7 @@
         <v>3197</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" s="3" t="s">
         <v>408</v>
       </c>
@@ -5772,7 +5764,7 @@
         <v>15186</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" s="3" t="s">
         <v>410</v>
       </c>
@@ -5798,7 +5790,7 @@
         <v>4645</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" s="3" t="s">
         <v>412</v>
       </c>
@@ -5824,7 +5816,7 @@
         <v>5055</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" s="3" t="s">
         <v>414</v>
       </c>
@@ -5850,7 +5842,7 @@
         <v>5510</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>416</v>
       </c>
@@ -5876,7 +5868,7 @@
         <v>5008</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>418</v>
       </c>
@@ -5902,7 +5894,7 @@
         <v>19224</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>420</v>
       </c>
@@ -5928,7 +5920,7 @@
         <v>12583</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>422</v>
       </c>
@@ -5954,7 +5946,7 @@
         <v>12084</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>449</v>
       </c>
@@ -5980,7 +5972,7 @@
         <v>24885</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
         <v>451</v>
       </c>
@@ -6006,7 +5998,7 @@
         <v>12825</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>453</v>
       </c>
@@ -6032,7 +6024,7 @@
         <v>6529</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A114" s="3" t="s">
         <v>455</v>
       </c>
@@ -6058,7 +6050,7 @@
         <v>5761</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A115" s="3" t="s">
         <v>457</v>
       </c>
@@ -6084,7 +6076,7 @@
         <v>6839</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A116" s="3" t="s">
         <v>459</v>
       </c>
@@ -6110,7 +6102,7 @@
         <v>12061</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A117" s="3" t="s">
         <v>461</v>
       </c>
@@ -6147,7 +6139,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6155,43 +6147,45 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C97BAFB-525F-42CF-A9A5-0D35515C64BF}">
-  <dimension ref="A1:S31"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="4" width="15.140625" customWidth="1"/>
+    <col min="4" max="5" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>477</v>
+        <v>524</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>507</v>
+        <v>1</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>485</v>
+        <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>487</v>
+        <v>525</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>526</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>482</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>483</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>484</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>502</v>
-      </c>
       <c r="H1" s="6" t="s">
-        <v>501</v>
-      </c>
-      <c r="I1" s="6"/>
+        <v>499</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>498</v>
+      </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
@@ -6202,32 +6196,35 @@
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
       <c r="S1" s="6"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="T1" s="6"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A2" s="6">
+        <v>160001</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="5" t="s">
-        <v>478</v>
-      </c>
       <c r="D2" s="5" t="s">
-        <v>486</v>
-      </c>
-      <c r="E2" s="6" t="str">
-        <f>TRIM(MID(D2, FIND(" ", D2) + 1, FIND("W", D2) - 1 - FIND(" ", D2)))</f>
+        <v>477</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>484</v>
+      </c>
+      <c r="F2" s="6" t="str">
+        <f>TRIM(MID(E2, FIND(" ", E2) + 1, FIND("W", E2) - 1 - FIND(" ", E2)))</f>
         <v>71°58'48"</v>
       </c>
-      <c r="F2" s="6" t="str">
-        <f>LEFT(D2, FIND("S", D2)-1)</f>
+      <c r="G2" s="6" t="str">
+        <f>LEFT(E2, FIND("S", E2)-1)</f>
         <v>13°31'00"</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="H2" s="6"/>
+      <c r="H2" s="6" t="s">
+        <v>497</v>
+      </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -6239,29 +6236,32 @@
       <c r="Q2" s="6"/>
       <c r="R2" s="6"/>
       <c r="S2" s="6"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="T2" s="6"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A3" s="6">
+        <v>160002</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>479</v>
-      </c>
       <c r="D3" s="5" t="s">
-        <v>488</v>
-      </c>
-      <c r="E3" s="6" t="str">
-        <f t="shared" ref="E3:E31" si="0">TRIM(MID(D3, FIND(" ", D3) + 1, FIND("W", D3) - 1 - FIND(" ", D3)))</f>
+        <v>478</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>485</v>
+      </c>
+      <c r="F3" s="6" t="str">
+        <f t="shared" ref="F3:F31" si="0">TRIM(MID(E3, FIND(" ", E3) + 1, FIND("W", E3) - 1 - FIND(" ", E3)))</f>
         <v>72°03'31"</v>
       </c>
-      <c r="F3" s="6" t="str">
-        <f t="shared" ref="F3:F31" si="1">LEFT(D3, FIND("S", D3)-1)</f>
+      <c r="G3" s="6" t="str">
+        <f t="shared" ref="G3:G31" si="1">LEFT(E3, FIND("S", E3)-1)</f>
         <v>13°35'04"</v>
       </c>
-      <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
@@ -6274,29 +6274,32 @@
       <c r="Q3" s="6"/>
       <c r="R3" s="6"/>
       <c r="S3" s="6"/>
-    </row>
-    <row r="4" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="T3" s="6"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A4" s="6">
+        <v>160003</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="C4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>479</v>
-      </c>
       <c r="D4" s="5" t="s">
-        <v>489</v>
-      </c>
-      <c r="E4" s="6" t="str">
+        <v>478</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>486</v>
+      </c>
+      <c r="F4" s="6" t="str">
         <f t="shared" si="0"/>
         <v>71°53'02"</v>
       </c>
-      <c r="F4" s="6" t="str">
+      <c r="G4" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°32'39"</v>
       </c>
-      <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
@@ -6309,29 +6312,32 @@
       <c r="Q4" s="6"/>
       <c r="R4" s="6"/>
       <c r="S4" s="6"/>
-    </row>
-    <row r="5" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="T4" s="6"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A5" s="6">
+        <v>160004</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="C5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>479</v>
-      </c>
       <c r="D5" s="5" t="s">
-        <v>490</v>
-      </c>
-      <c r="E5" s="6" t="str">
+        <v>478</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>487</v>
+      </c>
+      <c r="F5" s="6" t="str">
         <f t="shared" si="0"/>
         <v>71°56'14"</v>
       </c>
-      <c r="F5" s="6" t="str">
+      <c r="G5" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°31'48"</v>
       </c>
-      <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
       <c r="J5" s="6"/>
@@ -6344,29 +6350,32 @@
       <c r="Q5" s="6"/>
       <c r="R5" s="6"/>
       <c r="S5" s="6"/>
-    </row>
-    <row r="6" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="T5" s="6"/>
+    </row>
+    <row r="6" spans="1:20" ht="22" x14ac:dyDescent="0.2">
+      <c r="A6" s="6">
+        <v>160005</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="C6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>480</v>
-      </c>
       <c r="D6" s="5" t="s">
-        <v>491</v>
-      </c>
-      <c r="E6" s="6" t="str">
+        <v>479</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>488</v>
+      </c>
+      <c r="F6" s="6" t="str">
         <f t="shared" si="0"/>
         <v>71°58'59"</v>
       </c>
-      <c r="F6" s="6" t="str">
+      <c r="G6" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°31'31"</v>
       </c>
-      <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
@@ -6379,29 +6388,32 @@
       <c r="Q6" s="6"/>
       <c r="R6" s="6"/>
       <c r="S6" s="6"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="T6" s="6"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>160006</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="C7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>481</v>
-      </c>
       <c r="D7" s="5" t="s">
-        <v>492</v>
-      </c>
-      <c r="E7" s="6" t="str">
+        <v>480</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>489</v>
+      </c>
+      <c r="F7" s="6" t="str">
         <f t="shared" si="0"/>
         <v>71°49'38"</v>
       </c>
-      <c r="F7" s="6" t="str">
+      <c r="G7" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°34'11"</v>
       </c>
-      <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -6414,29 +6426,32 @@
       <c r="Q7" s="6"/>
       <c r="R7" s="6"/>
       <c r="S7" s="6"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="T7" s="6"/>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>160007</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="C8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>482</v>
-      </c>
       <c r="D8" s="5" t="s">
-        <v>493</v>
-      </c>
-      <c r="E8" s="6" t="str">
+        <v>481</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>490</v>
+      </c>
+      <c r="F8" s="6" t="str">
         <f t="shared" si="0"/>
         <v>71°58'14"</v>
       </c>
-      <c r="F8" s="6" t="str">
+      <c r="G8" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°31'12"</v>
       </c>
-      <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
@@ -6449,29 +6464,32 @@
       <c r="Q8" s="6"/>
       <c r="R8" s="6"/>
       <c r="S8" s="6"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="T8" s="6"/>
+    </row>
+    <row r="9" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A9" s="6">
+        <v>160008</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="C9" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>494</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>496</v>
-      </c>
-      <c r="E9" s="6" t="str">
+      <c r="D9" s="8" t="s">
+        <v>491</v>
+      </c>
+      <c r="E9" s="6" t="s">
+        <v>493</v>
+      </c>
+      <c r="F9" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°08'45"</v>
       </c>
-      <c r="F9" s="6" t="str">
+      <c r="G9" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°27'49"</v>
       </c>
-      <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -6484,29 +6502,32 @@
       <c r="Q9" s="6"/>
       <c r="R9" s="6"/>
       <c r="S9" s="6"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="T9" s="6"/>
+    </row>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A10" s="6">
+        <v>160009</v>
+      </c>
+      <c r="B10" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>497</v>
-      </c>
-      <c r="E10" s="6" t="str">
+      <c r="D10" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>494</v>
+      </c>
+      <c r="F10" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°18'01"</v>
       </c>
-      <c r="F10" s="6" t="str">
+      <c r="G10" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°27'26"</v>
       </c>
-      <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -6519,29 +6540,32 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="6"/>
       <c r="S10" s="6"/>
-    </row>
-    <row r="11" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="T10" s="6"/>
+    </row>
+    <row r="11" spans="1:20" ht="22" x14ac:dyDescent="0.2">
+      <c r="A11" s="6">
+        <v>160010</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="C11" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="8" t="s">
+        <v>492</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>495</v>
       </c>
-      <c r="D11" s="6" t="s">
-        <v>498</v>
-      </c>
-      <c r="E11" s="6" t="str">
+      <c r="F11" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°03'43"</v>
       </c>
-      <c r="F11" s="6" t="str">
+      <c r="G11" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°28'33"</v>
       </c>
-      <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -6554,32 +6578,35 @@
       <c r="Q11" s="6"/>
       <c r="R11" s="6"/>
       <c r="S11" s="6"/>
-    </row>
-    <row r="12" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="T11" s="6"/>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A12" s="6">
+        <v>160011</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="C12" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>499</v>
-      </c>
-      <c r="E12" s="6" t="str">
+      <c r="D12" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>496</v>
+      </c>
+      <c r="F12" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°13'54"</v>
       </c>
-      <c r="F12" s="6" t="str">
+      <c r="G12" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°37'41"</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="H12" s="6"/>
+      <c r="H12" s="6" t="s">
+        <v>497</v>
+      </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -6591,29 +6618,32 @@
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="T12" s="6"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A13" s="6">
+        <v>160012</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>503</v>
-      </c>
-      <c r="E13" s="6" t="str">
+      <c r="D13" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E13" s="6" t="s">
+        <v>500</v>
+      </c>
+      <c r="F13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°12'30"</v>
       </c>
-      <c r="F13" s="6" t="str">
+      <c r="G13" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°24'52"</v>
       </c>
-      <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -6626,29 +6656,32 @@
       <c r="Q13" s="6"/>
       <c r="R13" s="6"/>
       <c r="S13" s="6"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="T13" s="6"/>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A14" s="6">
+        <v>160013</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>504</v>
-      </c>
-      <c r="E14" s="6" t="str">
+      <c r="D14" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E14" s="6" t="s">
+        <v>501</v>
+      </c>
+      <c r="F14" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°26'35"</v>
       </c>
-      <c r="F14" s="6" t="str">
+      <c r="G14" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°28'46"</v>
       </c>
-      <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -6661,29 +6694,32 @@
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="T14" s="6"/>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A15" s="6">
+        <v>160014</v>
+      </c>
+      <c r="B15" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>505</v>
-      </c>
-      <c r="E15" s="6" t="str">
+      <c r="D15" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>502</v>
+      </c>
+      <c r="F15" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°31'17"</v>
       </c>
-      <c r="F15" s="6" t="str">
+      <c r="G15" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°28'55"</v>
       </c>
-      <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -6696,29 +6732,32 @@
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
+      <c r="T15" s="6"/>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A16" s="6">
+        <v>160015</v>
+      </c>
+      <c r="B16" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="C16" s="7" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>506</v>
-      </c>
-      <c r="E16" s="6" t="str">
+      <c r="D16" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>503</v>
+      </c>
+      <c r="F16" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°06'42"</v>
       </c>
-      <c r="F16" s="6" t="str">
+      <c r="G16" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°28'44"</v>
       </c>
-      <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -6731,29 +6770,32 @@
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
+      <c r="T16" s="6"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A17" s="6">
+        <v>160016</v>
+      </c>
+      <c r="B17" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C17" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>508</v>
-      </c>
-      <c r="E17" s="6" t="str">
+      <c r="D17" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>504</v>
+      </c>
+      <c r="F17" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°15'19"</v>
       </c>
-      <c r="F17" s="6" t="str">
+      <c r="G17" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°27'19"</v>
       </c>
-      <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -6766,29 +6808,32 @@
       <c r="Q17" s="6"/>
       <c r="R17" s="6"/>
       <c r="S17" s="6"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="T17" s="6"/>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A18" s="6">
+        <v>160017</v>
+      </c>
+      <c r="B18" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="C18" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="C18" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>512</v>
-      </c>
-      <c r="E18" s="6" t="str">
+      <c r="D18" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>508</v>
+      </c>
+      <c r="F18" s="6" t="str">
         <f t="shared" si="0"/>
         <v>71°57'20"</v>
       </c>
-      <c r="F18" s="6" t="str">
+      <c r="G18" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°19'16"</v>
       </c>
-      <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
       <c r="J18" s="6"/>
@@ -6801,29 +6846,32 @@
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="T18" s="6"/>
+    </row>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A19" s="6">
+        <v>160018</v>
+      </c>
+      <c r="B19" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B19" s="7" t="s">
+      <c r="C19" s="7" t="s">
         <v>110</v>
       </c>
-      <c r="C19" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>513</v>
-      </c>
-      <c r="E19" s="6" t="str">
+      <c r="D19" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E19" s="6" t="s">
+        <v>509</v>
+      </c>
+      <c r="F19" s="6" t="str">
         <f t="shared" si="0"/>
         <v>71°53'54"</v>
       </c>
-      <c r="F19" s="6" t="str">
+      <c r="G19" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°23'09"</v>
       </c>
-      <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
       <c r="J19" s="6"/>
@@ -6836,29 +6884,32 @@
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="T19" s="6"/>
+    </row>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A20" s="6">
+        <v>160019</v>
+      </c>
+      <c r="B20" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="C20" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>514</v>
-      </c>
-      <c r="E20" s="6" t="str">
+      <c r="D20" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>510</v>
+      </c>
+      <c r="F20" s="6" t="str">
         <f t="shared" si="0"/>
         <v>71°55'13"</v>
       </c>
-      <c r="F20" s="6" t="str">
+      <c r="G20" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°21'51"</v>
       </c>
-      <c r="G20" s="6"/>
       <c r="H20" s="6"/>
       <c r="I20" s="6"/>
       <c r="J20" s="6"/>
@@ -6871,32 +6922,35 @@
       <c r="Q20" s="6"/>
       <c r="R20" s="6"/>
       <c r="S20" s="6"/>
-    </row>
-    <row r="21" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="T20" s="6"/>
+    </row>
+    <row r="21" spans="1:20" ht="22" x14ac:dyDescent="0.2">
+      <c r="A21" s="6">
+        <v>160020</v>
+      </c>
+      <c r="B21" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="C21" s="7" t="s">
         <v>114</v>
       </c>
-      <c r="C21" s="8" t="s">
-        <v>509</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>515</v>
-      </c>
-      <c r="E21" s="6" t="str">
+      <c r="D21" s="8" t="s">
+        <v>505</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>511</v>
+      </c>
+      <c r="F21" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°02'36"</v>
       </c>
-      <c r="F21" s="6" t="str">
+      <c r="G21" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°06'12"</v>
       </c>
-      <c r="G21" s="6" t="s">
-        <v>500</v>
-      </c>
-      <c r="H21" s="6"/>
+      <c r="H21" s="6" t="s">
+        <v>497</v>
+      </c>
       <c r="I21" s="6"/>
       <c r="J21" s="6"/>
       <c r="K21" s="6"/>
@@ -6908,29 +6962,32 @@
       <c r="Q21" s="6"/>
       <c r="R21" s="6"/>
       <c r="S21" s="6"/>
-    </row>
-    <row r="22" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A22" s="6" t="s">
+      <c r="T21" s="6"/>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A22" s="6">
+        <v>160021</v>
+      </c>
+      <c r="B22" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="C22" s="7" t="s">
         <v>116</v>
       </c>
-      <c r="C22" s="8" t="s">
-        <v>510</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>516</v>
-      </c>
-      <c r="E22" s="6" t="str">
+      <c r="D22" s="8" t="s">
+        <v>506</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>512</v>
+      </c>
+      <c r="F22" s="6" t="str">
         <f t="shared" si="0"/>
         <v>71°51'01"</v>
       </c>
-      <c r="F22" s="6" t="str">
+      <c r="G22" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°25'15"</v>
       </c>
-      <c r="G22" s="6"/>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
@@ -6943,29 +7000,32 @@
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="T22" s="6"/>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A23" s="6">
+        <v>160022</v>
+      </c>
+      <c r="B23" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="C23" s="7" t="s">
         <v>118</v>
       </c>
-      <c r="C23" s="8" t="s">
-        <v>511</v>
-      </c>
-      <c r="D23" s="6" t="s">
-        <v>517</v>
-      </c>
-      <c r="E23" s="6" t="str">
+      <c r="D23" s="8" t="s">
+        <v>507</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>513</v>
+      </c>
+      <c r="F23" s="6" t="str">
         <f t="shared" si="0"/>
         <v>71°46'50"</v>
       </c>
-      <c r="F23" s="6" t="str">
+      <c r="G23" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°29'17"</v>
       </c>
-      <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
@@ -6978,182 +7038,223 @@
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="T23" s="6"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A24" s="6">
+        <v>160023</v>
+      </c>
+      <c r="B24" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="C24" s="7" t="s">
         <v>122</v>
       </c>
-      <c r="C24" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>518</v>
-      </c>
-      <c r="E24" s="6" t="str">
+      <c r="D24" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>514</v>
+      </c>
+      <c r="F24" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°03'20"</v>
       </c>
-      <c r="F24" s="6" t="str">
+      <c r="G24" s="6" t="str">
         <f t="shared" si="1"/>
         <v>12°48'39"</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+    </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A25" s="6">
+        <v>160024</v>
+      </c>
+      <c r="B25" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="C25" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="C25" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>521</v>
-      </c>
-      <c r="E25" s="6" t="str">
+      <c r="D25" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>517</v>
+      </c>
+      <c r="F25" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°06'52"</v>
       </c>
-      <c r="F25" s="6" t="str">
+      <c r="G25" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°18'20"</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A26" s="6">
+        <v>160025</v>
+      </c>
+      <c r="B26" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="C26" s="7" t="s">
         <v>452</v>
       </c>
-      <c r="C26" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>522</v>
-      </c>
-      <c r="E26" s="6" t="str">
+      <c r="D26" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>518</v>
+      </c>
+      <c r="F26" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°03'06"</v>
       </c>
-      <c r="F26" s="6" t="str">
+      <c r="G26" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°23'44"</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A27" s="6">
+        <v>160026</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="7" t="s">
         <v>454</v>
       </c>
-      <c r="C27" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>523</v>
-      </c>
-      <c r="E27" s="6" t="str">
+      <c r="D27" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>519</v>
+      </c>
+      <c r="F27" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°03'54"</v>
       </c>
-      <c r="F27" s="6" t="str">
+      <c r="G27" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°20'17"</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A28" s="6" t="s">
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+    </row>
+    <row r="28" spans="1:20" ht="22" x14ac:dyDescent="0.2">
+      <c r="A28" s="6">
+        <v>160027</v>
+      </c>
+      <c r="B28" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="C28" s="7" t="s">
         <v>456</v>
       </c>
-      <c r="C28" s="8" t="s">
-        <v>519</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>524</v>
-      </c>
-      <c r="E28" s="6" t="str">
+      <c r="D28" s="8" t="s">
+        <v>515</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>520</v>
+      </c>
+      <c r="F28" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°31'33"</v>
       </c>
-      <c r="F28" s="6" t="str">
+      <c r="G28" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°09'15"</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A29" s="6">
+        <v>160028</v>
+      </c>
+      <c r="B29" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B29" s="7" t="s">
+      <c r="C29" s="7" t="s">
         <v>458</v>
       </c>
-      <c r="C29" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>525</v>
-      </c>
-      <c r="E29" s="6" t="str">
+      <c r="D29" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>521</v>
+      </c>
+      <c r="F29" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°09'20"</v>
       </c>
-      <c r="F29" s="6" t="str">
+      <c r="G29" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°19'54"</v>
       </c>
-    </row>
-    <row r="30" spans="1:19" ht="18" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A30" s="6">
+        <v>160029</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="7" t="s">
         <v>460</v>
       </c>
-      <c r="C30" s="8" t="s">
-        <v>479</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>526</v>
-      </c>
-      <c r="E30" s="6" t="str">
+      <c r="D30" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>522</v>
+      </c>
+      <c r="F30" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°15'49"</v>
       </c>
-      <c r="F30" s="6" t="str">
+      <c r="G30" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°15'31"</v>
       </c>
-    </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31" s="6" t="s">
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
+      <c r="A31" s="6">
+        <v>160030</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>450</v>
       </c>
-      <c r="B31" s="7" t="s">
+      <c r="C31" s="7" t="s">
         <v>462</v>
       </c>
-      <c r="C31" s="8" t="s">
-        <v>520</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>527</v>
-      </c>
-      <c r="E31" s="6" t="str">
+      <c r="D31" s="8" t="s">
+        <v>516</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>523</v>
+      </c>
+      <c r="F31" s="6" t="str">
         <f t="shared" si="0"/>
         <v>72°05'00"</v>
       </c>
-      <c r="F31" s="6" t="str">
+      <c r="G31" s="6" t="str">
         <f t="shared" si="1"/>
         <v>13°19'15"</v>
       </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7166,7 +7267,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7178,7 +7279,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>